<commit_message>
feat: Sleep interruptions fix for scrapper
</commit_message>
<xml_diff>
--- a/Analysis/main_diseases_analysis_final.xlsx
+++ b/Analysis/main_diseases_analysis_final.xlsx
@@ -556,7 +556,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
@@ -903,7 +903,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -1488,7 +1488,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -3217,7 +3217,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="40" customWidth="1" min="2" max="2"/>
@@ -31691,7 +31691,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -33200,7 +33200,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -33873,7 +33873,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -34832,7 +34832,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -36517,7 +36517,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -37234,7 +37234,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -37533,7 +37533,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
@@ -38140,7 +38140,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>

</xml_diff>

<commit_message>
feat: Scrapper popus dodging.
</commit_message>
<xml_diff>
--- a/Analysis/main_diseases_analysis_final.xlsx
+++ b/Analysis/main_diseases_analysis_final.xlsx
@@ -89,7 +89,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -150,8 +150,14 @@
         <bgColor rgb="FFF8F9FA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8F9FA"/>
+        <bgColor rgb="00F8F9FA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,11 +195,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -232,6 +244,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +621,7 @@
       <selection activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="30" customWidth="1" style="15" min="1" max="1"/>
     <col width="15" customWidth="1" style="15" min="2" max="2"/>
@@ -950,7 +968,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -1534,7 +1552,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -3262,7 +3280,7 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="30" customWidth="1" style="15" min="1" max="1"/>
     <col width="40" customWidth="1" style="15" min="2" max="2"/>
@@ -3424,7 +3442,16 @@
           <t>https://www.drugs.com/5-htp-mood-and-stress.html</t>
         </is>
       </c>
-      <c r="G9" s="12" t="n"/>
+      <c r="G9" s="20">
+        <f>== 5-HTP Mood and Stress side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives, difficult breathing, swelling of your face, lips, tongue, or throat.
+Seek medical attention right away if you have symptoms of serotonin syndrome, such as: agitation, hallucinations, fever, sweating, shivering, fast heart rate, muscle stiffness, twitching, loss of coordination, nausea, vomiting, or diarrhea.
+Stop using 5-HTP Mood and Stress and call your healthcare provider at once if you have:
+slow heart rate, feeling like you might pass out;
+skin rash, bruising; or
+Common side effects of 5-HTP Mood and Stress may include:</f>
+        <v/>
+      </c>
       <c r="H9" s="10" t="n"/>
     </row>
     <row r="10" ht="409.5" customHeight="1" s="15">
@@ -3464,7 +3491,11 @@
           <t>https://www.drugs.com/a-g-profen.html</t>
         </is>
       </c>
-      <c r="G10" s="13" t="n"/>
+      <c r="G10" s="21" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for A-G Profen</t>
+        </is>
+      </c>
       <c r="H10" s="8" t="n"/>
     </row>
     <row r="11" ht="409.5" customHeight="1" s="15">
@@ -3504,7 +3535,15 @@
           <t>https://www.drugs.com/achromycin-v.html</t>
         </is>
       </c>
-      <c r="G11" s="12" t="n"/>
+      <c r="G11" s="20">
+        <f>== Achromycin V Side Effects ===
+Generic name: tetracycline
+Medically reviewed by Drugs.com. Last updated on Jun 23, 2025.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H11" s="10" t="n"/>
     </row>
     <row r="12" ht="16" customHeight="1" s="15">
@@ -3544,7 +3583,17 @@
           <t>https://www.drugs.com/actimmune.html</t>
         </is>
       </c>
-      <c r="G12" s="13" t="n"/>
+      <c r="G12" s="21">
+        <f>== Actimmune side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficulty breathing; swelling of your face, lips, tongue, or throat.
+Actimmune may cause serious side effects. Call your doctor at once if you have:
+confusion, hallucinations;
+a seizure (convulsions);
+low blood cell counts--fever, chills, flu-like symptoms, swollen gums, mouth sores, skin sores, easy bruising, unusual bleeding; or
+Your doses may be delayed or reduced if you have certain side effects.
+Common side effects of Actimmune may include:</f>
+        <v/>
+      </c>
       <c r="H12" s="8" t="n"/>
     </row>
     <row r="13" ht="16" customHeight="1" s="15">
@@ -3584,7 +3633,21 @@
           <t>https://www.drugs.com/activase.html</t>
         </is>
       </c>
-      <c r="G13" s="12" t="n"/>
+      <c r="G13" s="20">
+        <f>== Activase side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Activase increases your risk of bleeding, which can be severe or fatal. Call your doctor or seek emergency medical attention if you have bleeding that will not stop. Bleeding may occur from a surgical incision, or from the skin where a needle was inserted during a blood test or while receiving injectable medication. You may also have bleeding on the inside of your body, such as in your stomach or intestines, kidneys or bladder, brain, or within the muscles.
+Call your doctor or get emergency medical help if you have signs of bleeding, such as:
+sudden headache, feeling very weak or dizzy;
+bleeding gums, nosebleeds;
+easy bruising;
+bleeding from a wound, incision, catheter, or needle injection;
+bloody or tarry stools, coughing up blood or vomit that looks like coffee grounds;
+red or pink urine;
+heavy menstrual periods or abnormal vaginal bleeding; or
+Also call your doctor at once if you have:</f>
+        <v/>
+      </c>
       <c r="H13" s="10" t="n"/>
     </row>
     <row r="14" ht="16" customHeight="1" s="15">
@@ -3606,7 +3669,11 @@
           <t>https://www.drugs.com/addaprin.html</t>
         </is>
       </c>
-      <c r="G14" s="13" t="n"/>
+      <c r="G14" s="21" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for Addaprin</t>
+        </is>
+      </c>
       <c r="H14" s="8" t="n"/>
     </row>
     <row r="15" ht="16" customHeight="1" s="15">
@@ -3628,7 +3695,15 @@
           <t>https://www.drugs.com/adipex-p.html</t>
         </is>
       </c>
-      <c r="G15" s="12" t="n"/>
+      <c r="G15" s="20">
+        <f>== Adipex-P Side Effects ===
+Generic name: phentermine
+Medically reviewed by Drugs.com. Last updated on Nov 11, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H15" s="10" t="n"/>
     </row>
     <row r="16" ht="16" customHeight="1" s="15">
@@ -3646,7 +3721,20 @@
           <t>https://www.drugs.com/advair-hfa.html</t>
         </is>
       </c>
-      <c r="G16" s="13" t="n"/>
+      <c r="G16" s="21">
+        <f>== Advair HFA side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficulty breathing; swelling of your face, lips, tongue, or throat.
+Advair HFA may cause serious side effects. Call your doctor at once if you have:
+wheezing, choking, or other breathing problems after using this medicine;
+fever, chills, cough with mucus, feeling short of breath;
+chest pain, fast or irregular heartbeats, severe headache, pounding in your neck or ears;
+tremors, nervousness;
+blurred vision, tunnel vision, eye pain, or seeing halos around lights;
+high blood sugar--increased thirst, increased urination, dry mouth, fruity breath odor;
+signs of a hormonal disorder--worsening tiredness or weakness, feeling light-headed, nausea, vomiting.
+Common side effects of Advair HFA may include:</f>
+        <v/>
+      </c>
       <c r="H16" s="8" t="n"/>
     </row>
     <row r="17" ht="16" customHeight="1" s="15">
@@ -3664,7 +3752,11 @@
           <t>https://www.drugs.com/advil-children's.html</t>
         </is>
       </c>
-      <c r="G17" s="12" t="n"/>
+      <c r="G17" s="20" t="inlineStr">
+        <is>
+          <t>❌ Could not find main result for Advil Children's</t>
+        </is>
+      </c>
       <c r="H17" s="10" t="n"/>
     </row>
     <row r="18" ht="32" customHeight="1" s="15">
@@ -3682,7 +3774,11 @@
           <t>https://www.drugs.com/advil-infant's-concentrated-drops.html</t>
         </is>
       </c>
-      <c r="G18" s="13" t="n"/>
+      <c r="G18" s="21" t="inlineStr">
+        <is>
+          <t>❌ Could not find main result for Advil Infant's Concentrated Drops</t>
+        </is>
+      </c>
       <c r="H18" s="8" t="n"/>
     </row>
     <row r="19" ht="32" customHeight="1" s="15">
@@ -3700,7 +3796,16 @@
           <t>https://www.drugs.com/advil-junior-strength.html</t>
         </is>
       </c>
-      <c r="G19" s="12" t="n"/>
+      <c r="G19" s="20">
+        <f>== Advil Junior Strength Side Effects ===
+Advil Junior Strength
+Generic name: ibuprofen
+Medically reviewed by Drugs.com. Last updated on Jun 5, 2025.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H19" s="10" t="n"/>
     </row>
     <row r="20" ht="16" customHeight="1" s="15">
@@ -3718,7 +3823,15 @@
           <t>https://www.drugs.com/advil-liqui-gels.html</t>
         </is>
       </c>
-      <c r="G20" s="13" t="n"/>
+      <c r="G20" s="21">
+        <f>== Advil Liqui-Gels Side Effects ===
+Generic name: ibuprofen
+Medically reviewed by Drugs.com. Last updated on Jun 5, 2025.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H20" s="8" t="n"/>
     </row>
     <row r="21" ht="16" customHeight="1" s="15">
@@ -3736,7 +3849,22 @@
           <t>https://www.drugs.com/ala-tet.html</t>
         </is>
       </c>
-      <c r="G21" s="12" t="n"/>
+      <c r="G21" s="20">
+        <f>== Ala-Tet side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Ala-Tet may cause serious side effects. Call your doctor at once if you have:
+severe blistering, peeling, and red skin rash;
+fever, chills, body aches, flu symptoms;
+pale or yellowed skin, easy bruising or bleeding;
+any signs of a new infection.
+Common side effects of Ala-Tet may include:
+nausea, vomiting, diarrhea, upset stomach, loss of appetite;
+white patches or sores inside your mouth or on your lips;
+swollen tongue, black or "hairy" tongue, trouble swallowing;
+sores or swelling in your rectal or genital area; or
+vaginal itching or discharge.</f>
+        <v/>
+      </c>
       <c r="H21" s="10" t="n"/>
     </row>
     <row r="22" ht="16" customHeight="1" s="15">
@@ -3754,7 +3882,16 @@
           <t>https://www.drugs.com/altoprev.html</t>
         </is>
       </c>
-      <c r="G22" s="13" t="n"/>
+      <c r="G22" s="21">
+        <f>== Altoprev side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Altoprev can cause the breakdown of muscle tissue, which can lead to kidney failure. Call your doctor right away if you have unexplained muscle pain, tenderness, or weakness especially if you also have fever, unusual tiredness, or dark colored urine.
+Also call your doctor at once if you have:
+muscle weakness in your hips, shoulders, neck, and back;
+trouble lifting your arms, trouble climbing or standing;
+Common side effects of Altoprev may include:</f>
+        <v/>
+      </c>
       <c r="H22" s="8" t="n"/>
     </row>
     <row r="23" ht="16" customHeight="1" s="15">
@@ -3772,7 +3909,19 @@
           <t>https://www.drugs.com/amoclan.html</t>
         </is>
       </c>
-      <c r="G23" s="12" t="n"/>
+      <c r="G23" s="20">
+        <f>== Side Effects of Amoclan ===
+Along with its needed effects, a medicine may cause some unwanted effects. Although not all of these side effects may occur, if they do occur they may need medical attention.
+Check with your doctor immediately if any of the following side effects occur:
+Hives or welts
+itching
+itching of the vagina or genital area
+pain during sexual intercourse
+redness of the skin
+skin rash
+thick, white vaginal discharge with no odor or with a mild odor</f>
+        <v/>
+      </c>
       <c r="H23" s="10" t="n"/>
     </row>
     <row r="24" ht="16" customHeight="1" s="15">
@@ -3790,7 +3939,19 @@
           <t>https://www.drugs.com/anafranil.html</t>
         </is>
       </c>
-      <c r="G24" s="13" t="n"/>
+      <c r="G24" s="21">
+        <f>== Anafranil side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Seek medical treatment if you have a serious drug reaction that can affect many parts of your body. Symptoms may include: skin rash, fever, swollen glands, muscle aches, severe weakness, unusual bruising, or yellowing of your skin or eyes.
+Report any new or worsening symptoms to your doctor, such as: mood or behavior changes, anxiety, panic attacks, trouble sleeping, or if you feel impulsive, irritable, agitated, hostile, aggressive, restless, hyperactive (mentally or physically), more depressed, or have thoughts about suicide or hurting yourself.
+Anafranil may cause serious side effects. Call your doctor at once if you have:
+low sodium level --headache, confusion, slurred speech, severe weakness, vomiting, loss of coordination, feeling unsteady;
+blurred vision, tunnel vision, eye pain or swelling, or seeing halos around lights;
+confusion, extreme fear, thoughts of hurting yourself;
+pain or burning when you urinate; or
+a seizure (convulsions).</f>
+        <v/>
+      </c>
       <c r="H24" s="8" t="n"/>
     </row>
     <row r="25" ht="16" customHeight="1" s="15">
@@ -3808,7 +3969,19 @@
           <t>https://www.drugs.com/anaprox-ds.html</t>
         </is>
       </c>
-      <c r="G25" s="12" t="n"/>
+      <c r="G25" s="20">
+        <f>== Anaprox-DS side effects ===
+Get emergency medical help if you have signs of an allergic reaction (runny or stuffy nose, wheezing or trouble breathing, hives, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning eyes, skin pain, red or purple skin rash with blistering and peeling).
+Stop using Anaprox-DS and seek medical treatment if you have a serious drug reaction that can affect many parts of your body. Symptoms may include skin rash, fever, swollen glands, muscle aches, severe weakness, unusual bruising, or yellowing of your skin or eyes.
+Get emergency medical help if you have signs of a heart attack or stroke: chest pain spreading to your jaw or shoulder, sudden numbness or weakness on one side of the body, slurred speech, leg swelling, feeling short of breath.
+Anaprox-DS may cause serious side effects. Stop using Anaprox-DS and call your doctor at once if you have:
+shortness of breath (even with mild exertion);
+swelling or rapid weight gain;
+the first sign of any skin rash or blister, no matter how mild;
+liver problems--nausea, upper stomach pain, loss of appetite, dark urine, clay-colored stools, jaundice (yellowing of the skin or eyes);
+kidney problems--little or no urination, painful urination, swelling in your feet or ankles; or</f>
+        <v/>
+      </c>
       <c r="H25" s="10" t="n"/>
     </row>
     <row r="26" ht="16" customHeight="1" s="15">
@@ -3826,7 +3999,20 @@
           <t>https://www.drugs.com/antara.html</t>
         </is>
       </c>
-      <c r="G26" s="13" t="n"/>
+      <c r="G26" s="21">
+        <f>== Antara side effects ===
+Get emergency medical help if you have signs of an allergic reaction (hives, difficult breathing, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning in your eyes, skin pain, red or purple skin rash that spreads and causes blistering and peeling).
+In rare cases, Antara can cause a condition that results in the breakdown of skeletal muscle tissue, leading to kidney failure. Call your doctor right away if you have unexplained muscle pain, tenderness, or weakness especially if you also have fever, unusual tiredness, or dark colored urine.
+Also call your doctor at once if you have:
+sharp stomach pain spreading to your back or shoulder blade;
+loss of appetite, stomach pain just after eating a meal;
+jaundice (yellowing of the skin or eyes);
+fever, chills, weakness, sore throat, mouth sores, unusual bruising or bleeding;
+chest pain, sudden cough, wheezing, rapid breathing, coughing up blood; or
+swelling, warmth, or redness in an arm or leg.
+Common side effects of Antara may include:</f>
+        <v/>
+      </c>
       <c r="H26" s="8" t="n"/>
     </row>
     <row r="27" ht="16" customHeight="1" s="15">
@@ -3844,7 +4030,23 @@
           <t>https://www.drugs.com/apresoline.html</t>
         </is>
       </c>
-      <c r="G27" s="12" t="n"/>
+      <c r="G27" s="20">
+        <f>== Apresoline side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Apresoline may cause serious side effects. Call your doctor at once if you have:
+chest pain or pressure, pain spreading to your jaw or shoulder;
+fast or pounding heartbeats;
+a light-headed feeling, like you might pass out;
+numbness, tingling, or burning pain in your hands or feet;
+painful or difficult urination;
+little or no urination; or
+lupus-like syndrome--joint pain or swelling with fever, swollen glands, muscle aches, chest pain, vomiting, unusual thoughts or behavior, and patchy skin color.
+Common side effects of Apresoline may include:
+chest pain, fast heart rate;
+headache; or
+nausea, vomiting, diarrhea, loss of appetite.</f>
+        <v/>
+      </c>
       <c r="H27" s="10" t="n"/>
     </row>
     <row r="28" ht="16" customHeight="1" s="15">
@@ -3862,7 +4064,32 @@
           <t>https://www.drugs.com/aristospan.html</t>
         </is>
       </c>
-      <c r="G28" s="13" t="n"/>
+      <c r="G28" s="21">
+        <f>== Side Effects of Aristospan ===
+Along with its needed effects, a medicine may cause some unwanted effects. Although not all of these side effects may occur, if they do occur they may need medical attention.
+Check with your doctor or nurse immediately if any of the following side effects occur:
+Aggression
+agitation
+anxiety
+blurred vision
+decrease in the amount of urine
+dizziness
+fast, slow, pounding, or irregular heartbeat or pulse
+headache
+irritability
+mental depression
+mood changes
+nervousness
+noisy, rattling breathing
+numbness or tingling in the arms or legs
+pounding in the ears
+shortness of breath
+swelling of the fingers, hands, feet, or lower legs
+trouble thinking, speaking, or walking
+troubled breathing at rest
+weight gain</f>
+        <v/>
+      </c>
       <c r="H28" s="8" t="n"/>
     </row>
     <row r="29" ht="16" customHeight="1" s="15">
@@ -3880,7 +4107,18 @@
           <t>https://www.drugs.com/arthritis-pain.html</t>
         </is>
       </c>
-      <c r="G29" s="12" t="n"/>
+      <c r="G29" s="20">
+        <f>== Arthritis Pain side effects ===
+Platelet aggregation inhibitors
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Arthritis Pain may cause serious side effects. Stop using Arthritis Pain and call your doctor at once if you have:
+ringing in your ears, confusion, hallucinations, rapid breathing, seizure (convulsions);
+severe nausea, vomiting, or stomach pain;
+bloody or tarry stools, coughing up blood or vomit that looks like coffee grounds;
+fever lasting longer than 3 days; or
+swelling, or pain lasting longer than 10 days.</f>
+        <v/>
+      </c>
       <c r="H29" s="10" t="n"/>
     </row>
     <row r="30" ht="16" customHeight="1" s="15">
@@ -3898,7 +4136,11 @@
           <t>https://www.drugs.com/ascriptin.html</t>
         </is>
       </c>
-      <c r="G30" s="13" t="n"/>
+      <c r="G30" s="21" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for Ascriptin</t>
+        </is>
+      </c>
       <c r="H30" s="8" t="n"/>
     </row>
     <row r="31" ht="16" customHeight="1" s="15">
@@ -3916,7 +4158,11 @@
           <t>https://www.drugs.com/aspergum.html</t>
         </is>
       </c>
-      <c r="G31" s="12" t="n"/>
+      <c r="G31" s="20" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for Aspergum</t>
+        </is>
+      </c>
       <c r="H31" s="10" t="n"/>
     </row>
     <row r="32" ht="16" customHeight="1" s="15">
@@ -3934,7 +4180,18 @@
           <t>https://www.drugs.com/aspi-cor.html</t>
         </is>
       </c>
-      <c r="G32" s="13" t="n"/>
+      <c r="G32" s="21">
+        <f>== Aspi-Cor side effects ===
+Platelet aggregation inhibitors
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Aspi-Cor may cause serious side effects. Stop using Aspi-Cor and call your doctor at once if you have:
+ringing in your ears, confusion, hallucinations, rapid breathing, seizure (convulsions);
+severe nausea, vomiting, or stomach pain;
+bloody or tarry stools, coughing up blood or vomit that looks like coffee grounds;
+fever lasting longer than 3 days; or
+swelling, or pain lasting longer than 10 days.</f>
+        <v/>
+      </c>
       <c r="H32" s="8" t="n"/>
     </row>
     <row r="33" ht="16" customHeight="1" s="15">
@@ -3952,7 +4209,18 @@
           <t>https://www.drugs.com/aspir-low.html</t>
         </is>
       </c>
-      <c r="G33" s="12" t="n"/>
+      <c r="G33" s="20">
+        <f>== Aspir-Low side effects ===
+Platelet aggregation inhibitors
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Aspir-Low may cause serious side effects. Stop using Aspir-Low and call your doctor at once if you have:
+ringing in your ears, confusion, hallucinations, rapid breathing, seizure (convulsions);
+severe nausea, vomiting, or stomach pain;
+bloody or tarry stools, coughing up blood or vomit that looks like coffee grounds;
+fever lasting longer than 3 days; or
+swelling, or pain lasting longer than 10 days.</f>
+        <v/>
+      </c>
       <c r="H33" s="10" t="n"/>
     </row>
     <row r="34" ht="16" customHeight="1" s="15">
@@ -3970,7 +4238,11 @@
           <t>https://www.drugs.com/aspirtab.html</t>
         </is>
       </c>
-      <c r="G34" s="13" t="n"/>
+      <c r="G34" s="21" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for Aspirtab</t>
+        </is>
+      </c>
       <c r="H34" s="8" t="n"/>
     </row>
     <row r="35" ht="16" customHeight="1" s="15">
@@ -3988,7 +4260,17 @@
           <t>https://www.drugs.com/atorvaliq.html</t>
         </is>
       </c>
-      <c r="G35" s="12" t="n"/>
+      <c r="G35" s="20">
+        <f>== Atorvaliq side effects ===
+Get emergency medical help if you have signs of an allergic reaction (hives, difficult breathing, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning eyes, skin pain, red or purple skin rash with blistering and peeling).
+Atorvaliq can cause the breakdown of muscle tissue, which can lead to kidney failure. Call your doctor right away if you have unexplained muscle pain, tenderness, or weakness especially if you also have fever, unusual tiredness, or dark urine.
+Also call your doctor at once if you have:
+muscle weakness in your hips, shoulders, neck, and back;
+trouble lifting your arms, trouble climbing or standing;
+kidney problems--swelling, urinating less, feeling tired or short of breath; or
+high blood sugar--increased thirst, increased urination, dry mouth, fruity breath odor.</f>
+        <v/>
+      </c>
       <c r="H35" s="10" t="n"/>
     </row>
     <row r="36" ht="16" customHeight="1" s="15">
@@ -4006,7 +4288,17 @@
           <t>https://www.drugs.com/atrovent.html</t>
         </is>
       </c>
-      <c r="G36" s="13" t="n"/>
+      <c r="G36" s="21">
+        <f>== Atrovent HFA side effects ===
+Get emergency medical help if you have signs of an allergic reaction to Atrovent HFA: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+You may need to use a different bronchodilator medication if you have an allergic reaction to ipratropium.
+Call your doctor at once if you have:
+wheezing, choking, or other breathing problems after using this medicine;
+little or no urination;
+blurred vision, tunnel vision, eye pain, or seeing halos around lights; or
+worsened breathing problems.</f>
+        <v/>
+      </c>
       <c r="H36" s="8" t="n"/>
     </row>
     <row r="37" ht="16" customHeight="1" s="15">
@@ -4024,7 +4316,19 @@
           <t>https://www.drugs.com/augmentin-xr.html</t>
         </is>
       </c>
-      <c r="G37" s="12" t="n"/>
+      <c r="G37" s="20">
+        <f>== Side Effects of Augmentin XR ===
+Along with its needed effects, a medicine may cause some unwanted effects. Although not all of these side effects may occur, if they do occur they may need medical attention.
+Check with your doctor immediately if any of the following side effects occur:
+Hives or welts
+itching
+itching of the vagina or genital area
+pain during sexual intercourse
+redness of the skin
+skin rash
+thick, white vaginal discharge with no odor or with a mild odor</f>
+        <v/>
+      </c>
       <c r="H37" s="10" t="n"/>
     </row>
     <row r="38" ht="16" customHeight="1" s="15">
@@ -4042,7 +4346,15 @@
           <t>https://www.drugs.com/avtozma.html</t>
         </is>
       </c>
-      <c r="G38" s="13" t="n"/>
+      <c r="G38" s="21">
+        <f>== Avtozma Side Effects ===
+Generic name: tocilizumab
+Medically reviewed by Drugs.com. Last updated on Jun 25, 2025.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H38" s="8" t="n"/>
     </row>
     <row r="39" ht="32" customHeight="1" s="15">
@@ -4060,7 +4372,15 @@
           <t>https://www.drugs.com/azithromycin-dose-pack.html</t>
         </is>
       </c>
-      <c r="G39" s="12" t="n"/>
+      <c r="G39" s="20">
+        <f>== Azithromycin Dose Pack Side Effects ===
+Generic name: azithromycin
+Medically reviewed by Drugs.com. Last updated on Oct 16, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H39" s="10" t="n"/>
     </row>
     <row r="40" ht="16" customHeight="1" s="15">
@@ -4078,7 +4398,18 @@
           <t>https://www.drugs.com/azulfidine.html</t>
         </is>
       </c>
-      <c r="G40" s="13" t="n"/>
+      <c r="G40" s="21">
+        <f>== Azulfidine side effects ===
+Get emergency medical help if you have signs of an allergic reaction (hives, difficult breathing, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning eyes, skin pain, red or purple skin rash with blistering and peeling).
+Seek medical treatment if you have a serious drug reaction that can affect many parts of your body. Symptoms may include: skin rash, fever, swollen glands, muscle aches, severe weakness, unusual bruising, or yellowing of your skin or eyes.
+You may get infections more easily, even serious or fatal infections. Call your doctor right away if you have signs of infection such as:
+fever, chills, sore throat;
+mouth sores, red or swollen gums;
+pale skin, easy bruising, unusual bleeding; or
+chest discomfort, wheezing, dry cough or hack, rapid weight loss.
+Also call your doctor at once if you have:</f>
+        <v/>
+      </c>
       <c r="H40" s="8" t="n"/>
     </row>
     <row r="41" ht="16" customHeight="1" s="15">
@@ -4096,7 +4427,21 @@
           <t>https://www.drugs.com/b3-500-gr.html</t>
         </is>
       </c>
-      <c r="G41" s="12" t="n"/>
+      <c r="G41" s="20">
+        <f>== B3-500-Gr side effects ===
+Miscellaneous antihyperlipidemic agents
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+B3-500-Gr may cause serious side effects. Call your doctor at once if you have:
+heart attack symptoms--chest pain or pressure, pain spreading to your jaw or shoulder, nausea, sweating;
+high blood sugar--increased thirst, increased urination, dry mouth, fruity breath odor;
+unexplained muscle pain, tenderness or weakness;
+a light-headed feeling, like you might pass out;
+irregular heartbeats;
+severe warmth or redness under your skin;
+vision problems; or
+jaundice (yellowing of the skin or eyes).</f>
+        <v/>
+      </c>
       <c r="H41" s="10" t="n"/>
     </row>
     <row r="42" ht="16" customHeight="1" s="15">
@@ -4114,7 +4459,15 @@
           <t>https://www.drugs.com/bayer-aspirin.html</t>
         </is>
       </c>
-      <c r="G42" s="13" t="n"/>
+      <c r="G42" s="21">
+        <f>== Bayer Aspirin Side Effects ===
+Generic name: aspirin
+Medically reviewed by Drugs.com. Last updated on May 14, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H42" s="8" t="n"/>
     </row>
     <row r="43" ht="32" customHeight="1" s="15">
@@ -4132,7 +4485,15 @@
           <t>https://www.drugs.com/bayer-aspirin-extra-strength-plus.html</t>
         </is>
       </c>
-      <c r="G43" s="12" t="n"/>
+      <c r="G43" s="20">
+        <f>== Bayer Aspirin Extra Strength Plus Side Effects ===
+Generic name: aspirin
+Medically reviewed by Drugs.com. Last updated on May 14, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H43" s="10" t="n"/>
     </row>
     <row r="44" ht="16" customHeight="1" s="15">
@@ -4150,7 +4511,11 @@
           <t>https://www.drugs.com/belviq-xr.html</t>
         </is>
       </c>
-      <c r="G44" s="13" t="n"/>
+      <c r="G44" s="21" t="inlineStr">
+        <is>
+          <t>❌ No substantial side effects content found for Belviq XR</t>
+        </is>
+      </c>
       <c r="H44" s="8" t="n"/>
     </row>
     <row r="45" ht="16" customHeight="1" s="15">
@@ -4168,7 +4533,22 @@
           <t>https://www.drugs.com/brodspec.html</t>
         </is>
       </c>
-      <c r="G45" s="12" t="n"/>
+      <c r="G45" s="20">
+        <f>== Brodspec side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Brodspec may cause serious side effects. Call your doctor at once if you have:
+severe blistering, peeling, and red skin rash;
+fever, chills, body aches, flu symptoms;
+pale or yellowed skin, easy bruising or bleeding;
+any signs of a new infection.
+Common side effects of Brodspec may include:
+nausea, vomiting, diarrhea, upset stomach, loss of appetite;
+white patches or sores inside your mouth or on your lips;
+swollen tongue, black or "hairy" tongue, trouble swallowing;
+sores or swelling in your rectal or genital area; or
+vaginal itching or discharge.</f>
+        <v/>
+      </c>
       <c r="H45" s="10" t="n"/>
     </row>
     <row r="46" ht="16" customHeight="1" s="15">
@@ -4186,7 +4566,15 @@
           <t>https://www.drugs.com/celestone-soluspan.html</t>
         </is>
       </c>
-      <c r="G46" s="13" t="n"/>
+      <c r="G46" s="21">
+        <f>== Celestone Soluspan Side Effects ===
+Generic name: betamethasone
+Medically reviewed by Drugs.com. Last updated on Oct 28, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H46" s="8" t="n"/>
     </row>
     <row r="47" ht="16" customHeight="1" s="15">
@@ -4204,7 +4592,19 @@
           <t>https://www.drugs.com/chaparral.html</t>
         </is>
       </c>
-      <c r="G47" s="12" t="n"/>
+      <c r="G47" s="20">
+        <f>== Chaparral side effects ===
+Get emergency medical help if you have any of these signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Stop using chaparral and call your healthcare provider at once if you have:
+liver problems--nausea, upper stomach pain, itching, tired feeling, loss of appetite, dark urine, clay-colored stools, jaundice (yellowing of the skin or eyes); or
+Common side effects of chaparral may include:
+nausea, stomach pain;
+diarrhea, weight loss;
+fever;
+itching or rash (when used on the skin); or
+abnormal liver function tests.</f>
+        <v/>
+      </c>
       <c r="H47" s="10" t="n"/>
     </row>
     <row r="48" ht="16" customHeight="1" s="15">
@@ -4222,7 +4622,16 @@
           <t>https://www.drugs.com/chondroitin.html</t>
         </is>
       </c>
-      <c r="G48" s="13" t="n"/>
+      <c r="G48" s="21">
+        <f>== Chondroitin side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficult breathing; swelling of your face, lips, tongue, or throat.
+Although not all side effects are known, chondroitin is thought to be possibly safe when taken for up to 6 years.
+Stop using chondroitin and call your healthcare provider at once if you have:
+irregular heartbeats; or
+swelling in your legs.
+Common side effects of chondroitin may include:</f>
+        <v/>
+      </c>
       <c r="H48" s="8" t="n"/>
     </row>
     <row r="49" ht="16" customHeight="1" s="15">
@@ -4240,7 +4649,17 @@
           <t>https://www.drugs.com/cipro-i.v..html</t>
         </is>
       </c>
-      <c r="G49" s="12" t="n"/>
+      <c r="G49" s="20">
+        <f>== Cipro I.V. side effects ===
+Get emergency medical help if you have signs of an allergic reaction (hives, difficult breathing, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning in your eyes, skin pain, red or purple skin rash that spreads and causes blistering and peeling).
+Cipro I.V. can cause serious side effects, including tendon problems, side effects on your nerves (which may cause permanent nerve damage), serious mood or behavior changes (after just one dose), or low blood sugar (which can lead to coma).
+Stop using Cipro I.V. and call your doctor at once if you have:
+low blood sugar--headache, hunger, sweating, irritability, dizziness, nausea, fast heart rate, or feeling anxious or shaky;
+nerve symptoms in your hands, arms, legs, or feet--numbness, weakness, tingling, burning pain;
+serious mood or behavior changes--nervousness, confusion, agitation, paranoia, hallucinations, memory problems, trouble concentrating, thoughts of suicide; or
+In rare cases, Cipro I.V. may cause damage to your aorta, the main blood artery of the body. This could lead to dangerous bleeding or death. Get emergency medical help if you have severe and constant pain in your chest, stomach, or back.</f>
+        <v/>
+      </c>
       <c r="H49" s="10" t="n"/>
     </row>
     <row r="50" ht="16" customHeight="1" s="15">
@@ -4258,7 +4677,15 @@
           <t>https://www.drugs.com/cipro-xr.html</t>
         </is>
       </c>
-      <c r="G50" s="13" t="n"/>
+      <c r="G50" s="21">
+        <f>== Cipro XR Side Effects ===
+Generic name: ciprofloxacin
+Medically reviewed by Drugs.com. Last updated on Mar 20, 2024.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H50" s="8" t="n"/>
     </row>
     <row r="51" ht="16" customHeight="1" s="15">
@@ -4276,7 +4703,23 @@
           <t>https://www.drugs.com/claforan.html</t>
         </is>
       </c>
-      <c r="G51" s="12" t="n"/>
+      <c r="G51" s="20">
+        <f>== Claforan side effects ===
+Get emergency medical help if you have signs of an allergic reaction (hives, difficult breathing, swelling in your face or throat) or a severe skin reaction (fever, sore throat, burning in your eyes, skin pain, red or purple skin rash that spreads and causes blistering and peeling).
+Claforan may cause serious side effects. Call your doctor at once if you have:
+severe stomach pain, diarrhea that is watery or bloody (even if it occurs months after your last dose);
+burning, irritation, or skin changes where the injection was given;
+dark urine, jaundice (yellowing of the skin or eyes);
+a seizure;
+fever, chills, tiredness; or
+easy bruising, unusual bleeding, pale skin, cold hands and feet.
+Common side effects of Claforan may include:
+pain, bruising, swelling, or other irritation where the injection was given;
+diarrhea;
+fever; or
+rash, itching.</f>
+        <v/>
+      </c>
       <c r="H51" s="10" t="n"/>
     </row>
     <row r="52" ht="16" customHeight="1" s="15">
@@ -4294,7 +4737,14 @@
           <t>https://www.drugs.com/cleocin-hcl.html</t>
         </is>
       </c>
-      <c r="G52" s="13" t="n"/>
+      <c r="G52" s="21">
+        <f>== Cleocin Side Effects ===
+Generic name: clindamycin
+Medically reviewed by Drugs.com. Last updated on Mar 25, 2025.
+Serious side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H52" s="8" t="n"/>
     </row>
     <row r="53" ht="16" customHeight="1" s="15">
@@ -4312,7 +4762,15 @@
           <t>https://www.drugs.com/cleocin-pediatric.html</t>
         </is>
       </c>
-      <c r="G53" s="12" t="n"/>
+      <c r="G53" s="20">
+        <f>== Side Effects of Cleocin Pediatric ===
+Along with its needed effects, a medicine may cause some unwanted effects. Although not all of these side effects may occur, if they do occur they may need medical attention.
+Check with your doctor immediately if any of the following side effects occur:
+Cracks in the skin
+loss of heat from the body
+red, swollen skin scaly skin</f>
+        <v/>
+      </c>
       <c r="H53" s="10" t="n"/>
     </row>
     <row r="54" ht="16" customHeight="1" s="15">
@@ -4330,7 +4788,14 @@
           <t>https://www.drugs.com/cleocin-phosphate.html</t>
         </is>
       </c>
-      <c r="G54" s="13" t="n"/>
+      <c r="G54" s="21">
+        <f>== Cleocin Phosphate Side Effects ===
+Generic name: clindamycin
+Medically reviewed by Drugs.com. Last updated on Mar 25, 2025.
+Serious side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H54" s="8" t="n"/>
     </row>
     <row r="55" ht="16" customHeight="1" s="15">
@@ -4348,7 +4813,32 @@
           <t>https://www.drugs.com/clinacort.html</t>
         </is>
       </c>
-      <c r="G55" s="12" t="n"/>
+      <c r="G55" s="20">
+        <f>== Side Effects of Clinacort ===
+Along with its needed effects, a medicine may cause some unwanted effects. Although not all of these side effects may occur, if they do occur they may need medical attention.
+Check with your doctor or nurse immediately if any of the following side effects occur:
+Aggression
+agitation
+anxiety
+blurred vision
+decrease in the amount of urine
+dizziness
+fast, slow, pounding, or irregular heartbeat or pulse
+headache
+irritability
+mental depression
+mood changes
+nervousness
+noisy, rattling breathing
+numbness or tingling in the arms or legs
+pounding in the ears
+shortness of breath
+swelling of the fingers, hands, feet, or lower legs
+trouble thinking, speaking, or walking
+troubled breathing at rest
+weight gain</f>
+        <v/>
+      </c>
       <c r="H55" s="10" t="n"/>
     </row>
     <row r="56" ht="16" customHeight="1" s="15">
@@ -4366,7 +4856,18 @@
           <t>https://www.drugs.com/colestid.html</t>
         </is>
       </c>
-      <c r="G56" s="13" t="n"/>
+      <c r="G56" s="21">
+        <f>== Colestid side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficulty breathing; swelling of your face, lips, tongue, or throat.
+Colestid may cause serious side effects. Call your doctor at once if you have:
+trouble swallowing;
+severe constipation or stomach pain; or
+black, bloody, or tarry stools.
+Common side effects of Colestid may include:
+constipation; or
+hemorrhoids.</f>
+        <v/>
+      </c>
       <c r="H56" s="8" t="n"/>
     </row>
     <row r="57" ht="32" customHeight="1" s="15">
@@ -4384,7 +4885,15 @@
           <t>https://www.drugs.com/combivent-respimat.html</t>
         </is>
       </c>
-      <c r="G57" s="12" t="n"/>
+      <c r="G57" s="20">
+        <f>== Combivent Respimat Side Effects ===
+Generic name: albuterol / ipratropium
+Medically reviewed by Drugs.com. Last updated on Feb 12, 2025.
+Serious side effects
+Other side effects
+Professional info</f>
+        <v/>
+      </c>
       <c r="H57" s="10" t="n"/>
     </row>
     <row r="58" ht="16" customHeight="1" s="15">
@@ -4402,7 +4911,23 @@
           <t>https://www.drugs.com/corgard.html</t>
         </is>
       </c>
-      <c r="G58" s="13" t="n"/>
+      <c r="G58" s="21">
+        <f>== Corgard side effects ===
+Get emergency medical help if you have signs of an allergic reaction: hives; difficulty breathing; swelling of your face, lips, tongue, or throat.
+Corgard may cause serious side effects. Call your doctor at once if you have:
+a light-headed feeling, like you might pass out;
+slow heartbeats;
+shortness of breath (even with mild exertion), swelling, rapid weight gain; or
+bronchospasm (wheezing, chest tightness, trouble breathing).
+Common side effects of Corgard may include:
+numbness or cold feeling in your hands or feet;
+dizziness;
+feeling tired;
+upset stomach, vomiting, diarrhea, constipation;
+vision problems; or
+mood changes, confusion, memory problems.</f>
+        <v/>
+      </c>
       <c r="H58" s="8" t="n"/>
     </row>
     <row r="59" ht="16" customHeight="1" s="15">
@@ -9471,7 +9996,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -10979,7 +11504,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -11651,7 +12176,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -12609,7 +13134,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -14293,7 +14818,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -15009,7 +15534,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -15307,7 +15832,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>
@@ -15913,7 +16438,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" style="15" min="1" max="1"/>
     <col width="50" customWidth="1" style="15" min="2" max="2"/>

</xml_diff>

<commit_message>
chore: new column in the excel.
</commit_message>
<xml_diff>
--- a/Analysis/main_diseases_analysis_final.xlsx
+++ b/Analysis/main_diseases_analysis_final.xlsx
@@ -3211,10 +3211,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="40" customWidth="1" min="2" max="2"/>
-    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
     <col width="35" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -3275,22 +3275,22 @@
       </c>
       <c r="B8" s="13" t="inlineStr">
         <is>
+          <t>WHAT IS</t>
+        </is>
+      </c>
+      <c r="C8" s="13" t="inlineStr">
+        <is>
           <t>SIDE EFFECTS</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="D8" s="13" t="inlineStr">
         <is>
           <t>CALL A DOCTOR IF</t>
         </is>
       </c>
-      <c r="D8" s="13" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>GO TO ER IF</t>
-        </is>
-      </c>
-      <c r="E8" s="13" t="inlineStr">
-        <is>
-          <t>DOSAGE</t>
         </is>
       </c>
     </row>
@@ -6915,7 +6915,7 @@
     <row r="340">
       <c r="A340" s="16" t="inlineStr">
         <is>
-          <t>Next Steps: Populate columns B-E with FDA/Drugs.com data</t>
+          <t>Next Steps: Populate columns B-E with medication data (What Is, Side Effects, Call Doctor, Go to ER)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Delete a couple of unused files
</commit_message>
<xml_diff>
--- a/Analysis/main_diseases_analysis_final.xlsx
+++ b/Analysis/main_diseases_analysis_final.xlsx
@@ -2407,10 +2407,26 @@
           <t>5-HTP Mood and Stress</t>
         </is>
       </c>
-      <c r="B9" s="15" t="inlineStr"/>
-      <c r="C9" s="15" t="inlineStr"/>
-      <c r="D9" s="15" t="inlineStr"/>
-      <c r="E9" s="15" t="inlineStr"/>
+      <c r="B9" s="15" t="inlineStr">
+        <is>
+          <t>5-HTP Mood and Stress is a natural product used in alternative medicine. While it's been shown to be possibly effective in treating depression, its efficacy in other uses including anxiety, Down syndrome, alcohol withdrawal, Alzheimer's disease, headaches, attention deficit disorder, muscle spasms in the mouth, fibromyalgia, premenstrual syndrome, seizures, weight loss, Parkinson's disease, and sleep disorders lacks sufficient research to confirm effectiveness. This information is for educational purposes only and is not intended for medical advice, diagnosis, or treatment.</t>
+        </is>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>* Allergic reaction: hives, difficult breathing, swelling of face, lips, tongue, or throat. * Serotonin syndrome: agitation, hallucinations, fever, sweating, shivering, fast heart rate, muscle stiffness, twitching, loss of coordination, nausea, vomiting, diarrhea. * Skin rash * Bruising * Headache * Dizziness * Weakness * Severe vomiting * Stomach pain * Heartburn * Diarrhea * Constipation * Slow heart rate * Feeling like you might pass out * Racing thoughts * Increased energy * Decreased need for sleep * Risk-taking behavior * Agitation * Talkativeness</t>
+        </is>
+      </c>
+      <c r="D9" s="15" t="inlineStr">
+        <is>
+          <t>* Your symptoms do not improve or worsen. * You are considering surgery (stop taking 5-HTP at least 2 weeks prior). * You experience any of the listed side effects. * You are using stimulant medicine, opioid medicine, herbal products, or medicine for depression, mental illness, Parkinson's disease, migraine headaches, serious infections, or prevention of nausea and vomiting (due to potential serotonin syndrome interaction).</t>
+        </is>
+      </c>
+      <c r="E9" s="15" t="inlineStr">
+        <is>
+          <t>* You have signs of an allergic reaction (hives, difficult breathing, swelling of face, lips, tongue, or throat). * You have symptoms of serotonin syndrome (agitation, hallucinations, fever, sweating, shivering, fast heart rate, muscle stiffness, twitching, loss of coordination, nausea, vomiting, or diarrhea). * You experience an overdose (contact Poison Help line at 1-800-222-1222).</t>
+        </is>
+      </c>
       <c r="F9" s="15" t="inlineStr">
         <is>
           <t>Depression (major depressive disorder)</t>
@@ -2423,10 +2439,26 @@
           <t>A-G Profen</t>
         </is>
       </c>
-      <c r="B10" s="11" t="inlineStr"/>
-      <c r="C10" s="11" t="inlineStr"/>
-      <c r="D10" s="11" t="inlineStr"/>
-      <c r="E10" s="11" t="inlineStr"/>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>A-G Profen (presumed to be an ibuprofen-based medication) is a nonsteroidal anti-inflammatory drug (NSAID) used to treat mild to moderate pain and the symptoms of arthritis (osteoarthritis, rheumatoid arthritis, or juvenile arthritis), such as inflammation, swelling, stiffness, and joint pain. It can also be used to treat fever and menstrual cramps, as directed by a doctor. This medication does not cure arthritis; its effects last only as long as it is taken. Dosage for children under 2 years old is determined by body weight and temperature and should be prescribed by a doctor.</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>* Increased risk of serious cardiovascular thrombotic events, myocardial infarction, and stroke (potentially fatal) * Increased risk of serious gastrointestinal adverse events (especially in the elderly), including bleeding, ulceration, and perforation of the stomach or intestines (potentially fatal) * Bleeding in the stomach or intestines (may occur without warning signs) * Serious skin reactions (blistering, peeling, loosening of skin, chills, cough, diarrhea, fever, itching, joint or muscle pain, red skin lesions, sore throat, sores, ulcers, white spots in mouth or on lips, unusual tiredness or weakness) * Edema (fluid retention or body swelling) * Stomach or intestinal ulcers or bleeding * Nausea * Vomiting * Abdominal pain * Acid or sour stomach * Belching * Bloating * Cloudy urine * Decrease in amount of urine * Decrease in urine output or decrease in urine-concentrating ability * Diarrhea * Difficulty having a bowel movement * Excess air or gas in stomach or intestines * Full feeling * Heartburn * Indigestion * Itching skin * Pain or discomfort in chest, upper stomach, or throat * Pale skin * Passing gas * Noisy, rattling breathing * Rash with flat lesions or small raised lesions on the skin * Shortness of breath * Swelling of face, fingers, hands, feet, lower legs, or ankles * Troubled breathing at rest * Troubled breathing with exertion * Unusual bleeding or bruising * Unusual tiredness or weakness * Weight gain * Anaphylaxis (rare, but may be more common in patients allergic to aspirin or other NSAIDs): very fast or irregular breathing, gasping for breath, wheezing, fainting, changes in skin color of the face, very fast but irregular heartbeat or pulse, hive-like swellings on the skin, puffiness or swelling of the eyelids or around the eyes. * Symptoms of meningitis (fever, headache, nausea, vomiting, stiff neck or back) * Swelling of the face, fingers, feet, and/or lower legs * Severe stomach pain * Black, tarry stools * Vomiting of blood or material that... [truncated]</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>* You experience any unusual or allergic reaction to the medicine or any other medicine. * You have any other allergies (foods, dyes, preservatives, or animals). * You have age-related kidney problems (especially if elderly). * You are taking other medications (especially steroids or blood thinners). * You experience any of the following symptoms: blistering, peeling, loosening of skin, chills, cough, diarrhea, fever, itching, joint or muscle pain, red skin lesions, sore throat, sores, ulcers, white spots in mouth or on lips, unusual tiredness or weakness. * You notice swelling of the face, fingers, feet, and/or lower legs; severe stomach pain, black, tarry stools, and/or vomiting of blood or material that looks like coffee grounds; unusual weight gain; yellow skin or eyes; decreased urination; bleeding or bruising; and/or skin rash. * You notice signs of serious heart problems such as chest pain, tightness in chest, fast or irregular heartbeat, unusual flushing or warmth of skin, weakness, or slurring of speech. * You develop fever, headache, nausea, vomiting, and stiff neck or back. * You experience any of the listed side effects (see SIDE EFFECTS section).</t>
+        </is>
+      </c>
+      <c r="E10" s="11" t="inlineStr">
+        <is>
+          <t>* You experience anaphylaxis: very fast or irregular breathing, gasping for breath, wheezing, fainting, changes in skin color of the face, very fast but irregular heartbeat or pulse, hive-like swellings on the skin, puffiness or swelling of the eyelids or around the eyes.</t>
+        </is>
+      </c>
       <c r="F10" s="11" t="inlineStr">
         <is>
           <t>Arthritis</t>
@@ -2439,10 +2471,26 @@
           <t>Achromycin V</t>
         </is>
       </c>
-      <c r="B11" s="15" t="inlineStr"/>
-      <c r="C11" s="15" t="inlineStr"/>
-      <c r="D11" s="15" t="inlineStr"/>
-      <c r="E11" s="15" t="inlineStr"/>
+      <c r="B11" s="15" t="inlineStr">
+        <is>
+          <t>Achromycin V (Tetracycline HCl Capsules, USP) is an antibiotic in the tetracycline class. It works by inhibiting protein synthesis in bacteria, making it effective against a wide range of gram-negative and gram-positive organisms. It's used to treat various bacterial infections, including those of the upper and lower respiratory tract, skin and soft tissues, urinary tract, and infections caused by specific bacteria like *Chlamydia trachomatis*, *Rickettsia*, and others. It's also used as an alternative to penicillin in certain infections when penicillin is contraindicated. Importantly, Achromycin V should only be used to treat infections proven or strongly suspected to be bacterial. It is not effective against viral infections.</t>
+        </is>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>* **Gastrointestinal:** anorexia, nausea, epigastric distress, vomiting, diarrhea, glossitis, black hairy tongue, dysphagia, enterocolitis, inflammatory lesions (with monilial overgrowth) in the anogenital region. * **Teeth:** permanent discoloration (yellow-gray-brown), enamel hypoplasia (especially during tooth development last half of pregnancy, infancy, and childhood to age 8). * **Skin:** maculopapular and erythrematous rashes, exfoliative dermatitis (uncommon), onycholysis, discoloration of nails, photosensitivity (exaggerated sunburn reaction). * **Hypersensitivity Reactions:** urticaria, angioneurotic edema, anaphylaxis, anaphylactoid purpura, pericarditis, exacerbation of systemic lupus erythematosus, serum sickness-like reactions (fever, rash, arthralgia). * **Other:** bulging fontanels in infants, intracranial pressure in adults, decreased fibula growth rate in premature infants (reversible upon discontinuation), overgrowth of nonsusceptible organisms (including fungi superinfection).</t>
+        </is>
+      </c>
+      <c r="D11" s="15" t="inlineStr">
+        <is>
+          <t>* You experience any of the listed side effects. * You develop a superinfection (overgrowth of nonsusceptible organisms). * You have renal impairment and need dosage adjustment. * You are pregnant, breastfeeding, or considering becoming pregnant (due to potential for tooth discoloration and other effects on the developing fetus/infant). * You are treating a streptococcal infection; treatment should last at least 10 days. * You have symptoms that don't improve or worsen after 24-48 hours of treatment. * You have an allergic reaction. * You develop skin erythema (redness) from photosensitivity.</t>
+        </is>
+      </c>
+      <c r="E11" s="15" t="inlineStr">
+        <is>
+          <t>* You experience a severe allergic reaction (anaphylaxis, angioedema). * You experience severe or life-threatening symptoms (e.g., difficulty breathing, severe rash). * No specific information regarding situations requiring immediate ER visit is explicitly stated but severe allergic reactions and life-threatening symptoms would warrant immediate medical attention.</t>
+        </is>
+      </c>
       <c r="F11" s="15" t="inlineStr">
         <is>
           <t>Arthritis</t>
@@ -2455,10 +2503,26 @@
           <t>Actimmune</t>
         </is>
       </c>
-      <c r="B12" s="11" t="inlineStr"/>
-      <c r="C12" s="11" t="inlineStr"/>
-      <c r="D12" s="11" t="inlineStr"/>
-      <c r="E12" s="11" t="inlineStr"/>
+      <c r="B12" s="11" t="inlineStr">
+        <is>
+          <t>Actimmune is a medication made from human proteins (interferons) that help the body fight viral infections. It's primarily used to prevent serious infections in individuals with chronic granulomatous disease and to slow the progression of malignant osteopetrosis (a bone disorder).</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
+        <is>
+          <t>* Allergic reactions: hives, difficulty breathing, swelling of the face, lips, tongue, or throat * Seizures (convulsions) * Low blood cell counts: fever, chills, flu-like symptoms, swollen gums, mouth sores, skin sores, easy bruising, unusual bleeding * Kidney problems: little or no urination, painful or difficult urination, swelling in the feet or ankles, feeling tired or short of breath * Confusion * Hallucinations * Increased risk of infection due to lowered blood cell counts * Increased risk of bleeding due to lowered blood cell counts * Dizziness * Loss of balance or coordination * Flu-like symptoms (can be associated with low blood cell counts or overdose)</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>* You experience unusual bruising or bleeding. * You experience signs of infection (fever, chills, body aches). * You have any of the following serious side effects: * Seizures (convulsions) * Low blood cell counts (with associated symptoms) * Kidney problems (with associated symptoms) * Confusion * Hallucinations * You experience any side effects that concern you.</t>
+        </is>
+      </c>
+      <c r="E12" s="11" t="inlineStr">
+        <is>
+          <t>* You have signs of an allergic reaction: hives, difficulty breathing, swelling of your face, lips, tongue, or throat.</t>
+        </is>
+      </c>
       <c r="F12" s="11" t="inlineStr">
         <is>
           <t>Chronic kidney disease</t>
@@ -2471,10 +2535,26 @@
           <t>Activase</t>
         </is>
       </c>
-      <c r="B13" s="15" t="inlineStr"/>
-      <c r="C13" s="15" t="inlineStr"/>
-      <c r="D13" s="15" t="inlineStr"/>
-      <c r="E13" s="15" t="inlineStr"/>
+      <c r="B13" s="15" t="inlineStr">
+        <is>
+          <t>Activase is a prescription medication. While the provided text does not specify its use, it strongly implies it's a medication with a significant risk of bleeding as a side effect. Further information regarding its specific indications and uses would be needed from additional reliable sources.</t>
+        </is>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>* Allergic reaction: hives, difficult breathing, swelling of the face, lips, tongue, or throat. * Bleeding (internal and external): This can be severe or fatal. Bleeding may occur from surgical incisions, needle insertion sites, or internally (stomach, intestines, kidneys, bladder, brain, muscles). * Sudden headache * Feeling very weak or dizzy * Bleeding gums * Nosebleeds * Easy bruising * Bleeding from a wound, incision, catheter, or needle injection * Bloody or tarry stools * Coughing up blood or vomit that looks like coffee grounds * Red or pink urine * Heavy menstrual periods or abnormal vaginal bleeding * Sudden numbness or weakness (especially on one side of the body) * Slurred speech * Problems with vision or balance * Chest pain or heavy feeling, pain spreading to the jaw or shoulder, nausea, sweating, general ill feeling * Swelling * Rapid weight gain * Little or no urination * Severe stomach pain * Nausea and vomiting * Increased blood pressure (severe headache, blurred vision, pounding in your neck or ears, anxiety, nosebleed) * Pancreatitis (severe pain in your upper stomach spreading to your back, nausea and vomiting)</t>
+        </is>
+      </c>
+      <c r="D13" s="15" t="inlineStr">
+        <is>
+          <t>* You experience any signs of bleeding (as listed above). * You have chest pain or heavy feeling, pain spreading to the jaw or shoulder, nausea, sweating, general ill feeling. * You have swelling, rapid weight gain, or little or no urination. * You have severe stomach pain, nausea, and vomiting. * You have increased blood pressure symptoms (severe headache, blurred vision, pounding in your neck or ears, anxiety, nosebleed). * You experience pancreatitis symptoms (severe pain in your upper stomach spreading to your back, nausea and vomiting).</t>
+        </is>
+      </c>
+      <c r="E13" s="15" t="inlineStr">
+        <is>
+          <t>* You have signs of an allergic reaction (hives, difficult breathing, swelling of your face, lips, tongue, or throat). * You have bleeding that will not stop.</t>
+        </is>
+      </c>
       <c r="F13" s="15" t="inlineStr">
         <is>
           <t>Stroke</t>
@@ -7633,6 +7713,7 @@
         </is>
       </c>
     </row>
+    <row r="336"/>
     <row r="337">
       <c r="A337" s="16" t="inlineStr">
         <is>
@@ -8556,8 +8637,8 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A82:F82"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A82:F82"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>